<commit_message>
database ver1 - dont have stored-procedure
</commit_message>
<xml_diff>
--- a/TaskNote.xlsx
+++ b/TaskNote.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Tuần 1</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Tuần 8</t>
-  </si>
-  <si>
-    <t>-Code Front-end with React</t>
   </si>
   <si>
     <t>- Hoàn thành khảo sát hiện trạng (3 trang)
@@ -83,6 +80,51 @@
   </si>
   <si>
     <t>- Chờ chuyển sang .jsx</t>
+  </si>
+  <si>
+    <t>Tuần 9</t>
+  </si>
+  <si>
+    <t>-Code UI</t>
+  </si>
+  <si>
+    <t>-Create database with MySQL
+-Code Front-end with React</t>
+  </si>
+  <si>
+    <t>- xong CSDL
+'-xong UI and Admin page</t>
+  </si>
+  <si>
+    <t>Tuần 10</t>
+  </si>
+  <si>
+    <t>-Code Back-end API full
+-Code Front-end full page</t>
+  </si>
+  <si>
+    <t>Tuần 11</t>
+  </si>
+  <si>
+    <t>-Code hoàn thiện</t>
+  </si>
+  <si>
+    <t>-Database hoàn thiện</t>
+  </si>
+  <si>
+    <t>Tuần 12</t>
+  </si>
+  <si>
+    <t>Tuần 13</t>
+  </si>
+  <si>
+    <t>-Báo cáo hoàn thiện</t>
+  </si>
+  <si>
+    <t>Tuần 14</t>
+  </si>
+  <si>
+    <t>-Xong!</t>
   </si>
 </sst>
 </file>
@@ -450,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -502,7 +544,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -517,7 +559,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -529,28 +571,38 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
@@ -558,8 +610,12 @@
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
@@ -567,8 +623,12 @@
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
@@ -576,8 +636,12 @@
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
@@ -585,8 +649,12 @@
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>

</xml_diff>